<commit_message>
move to single file
</commit_message>
<xml_diff>
--- a/doc/instruction.xlsx
+++ b/doc/instruction.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Kele\Workspaces\kv32\doc\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0CED86E2-2A24-40CD-979B-3DDCFA8DC66F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7DDECA2-6E5B-42CD-B41F-2ACE5A08CED2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="296" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" tabRatio="296" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="775" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="795" uniqueCount="236">
   <si>
     <t>31:25</t>
   </si>
@@ -724,6 +724,27 @@
   </si>
   <si>
     <t>or    rd,  rs1, rs10</t>
+  </si>
+  <si>
+    <t>Number</t>
+  </si>
+  <si>
+    <t>Zicsr (1 type, 1 opcode, 6 instructions)</t>
+  </si>
+  <si>
+    <t>RV32I (8 types, 11 opcodes, 40 instructions)</t>
+  </si>
+  <si>
+    <t>csr[11:0]</t>
+  </si>
+  <si>
+    <t>opcode</t>
+  </si>
+  <si>
+    <t>Opcde</t>
+  </si>
+  <si>
+    <t>imm[11:0], funct7</t>
   </si>
 </sst>
 </file>
@@ -766,7 +787,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="14">
+  <fills count="16">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -845,8 +866,20 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="4">
+  <borders count="5">
     <border>
       <left/>
       <right/>
@@ -895,11 +928,20 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="96">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -991,13 +1033,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -1011,12 +1058,44 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="14" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="2" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="11" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="15" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1299,35 +1378,35 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B2:Q49"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A11" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="N37" sqref="N37"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="4" max="4" width="12.5703125" customWidth="1"/>
-    <col min="8" max="12" width="12.85546875" customWidth="1"/>
-    <col min="13" max="13" width="12.28515625" customWidth="1"/>
-    <col min="14" max="14" width="30.5703125" customWidth="1"/>
-    <col min="15" max="15" width="32.7109375" customWidth="1"/>
-    <col min="16" max="16" width="46.140625" customWidth="1"/>
-    <col min="17" max="17" width="19.7109375" customWidth="1"/>
+    <col min="4" max="4" width="12.5546875" customWidth="1"/>
+    <col min="8" max="12" width="12.88671875" customWidth="1"/>
+    <col min="13" max="13" width="12.33203125" customWidth="1"/>
+    <col min="14" max="14" width="30.5546875" customWidth="1"/>
+    <col min="15" max="15" width="32.6640625" customWidth="1"/>
+    <col min="16" max="16" width="46.109375" customWidth="1"/>
+    <col min="17" max="17" width="19.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:17" x14ac:dyDescent="0.25">
-      <c r="B2" s="76" t="s">
+    <row r="2" spans="2:17" x14ac:dyDescent="0.3">
+      <c r="B2" s="74" t="s">
         <v>186</v>
       </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-    </row>
-    <row r="4" spans="2:17" x14ac:dyDescent="0.25">
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+    </row>
+    <row r="4" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B4" s="57"/>
       <c r="C4" s="5" t="s">
         <v>26</v>
@@ -1375,7 +1454,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="5" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B5" s="75">
         <v>5</v>
       </c>
@@ -1423,7 +1502,7 @@
       </c>
       <c r="Q5" s="11"/>
     </row>
-    <row r="6" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B6" s="75"/>
       <c r="C6" s="64" t="s">
         <v>17</v>
@@ -1469,7 +1548,7 @@
       </c>
       <c r="Q6" s="11"/>
     </row>
-    <row r="7" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B7" s="75"/>
       <c r="C7" s="64" t="s">
         <v>17</v>
@@ -1515,7 +1594,7 @@
       </c>
       <c r="Q7" s="11"/>
     </row>
-    <row r="8" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B8" s="75"/>
       <c r="C8" s="64" t="s">
         <v>17</v>
@@ -1561,7 +1640,7 @@
       </c>
       <c r="Q8" s="11"/>
     </row>
-    <row r="9" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B9" s="75"/>
       <c r="C9" s="64" t="s">
         <v>17</v>
@@ -1607,7 +1686,7 @@
       </c>
       <c r="Q9" s="11"/>
     </row>
-    <row r="10" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B10" s="75">
         <v>3</v>
       </c>
@@ -1655,7 +1734,7 @@
       </c>
       <c r="Q10" s="14"/>
     </row>
-    <row r="11" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="11" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B11" s="75"/>
       <c r="C11" s="64" t="s">
         <v>18</v>
@@ -1701,7 +1780,7 @@
       </c>
       <c r="Q11" s="14"/>
     </row>
-    <row r="12" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B12" s="75"/>
       <c r="C12" s="64" t="s">
         <v>18</v>
@@ -1747,7 +1826,7 @@
       </c>
       <c r="Q12" s="14"/>
     </row>
-    <row r="13" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B13" s="75">
         <v>6</v>
       </c>
@@ -1795,7 +1874,7 @@
       </c>
       <c r="Q13" s="32"/>
     </row>
-    <row r="14" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B14" s="75"/>
       <c r="C14" s="64" t="s">
         <v>19</v>
@@ -1841,7 +1920,7 @@
       </c>
       <c r="Q14" s="32"/>
     </row>
-    <row r="15" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B15" s="75"/>
       <c r="C15" s="64" t="s">
         <v>19</v>
@@ -1887,7 +1966,7 @@
       </c>
       <c r="Q15" s="32"/>
     </row>
-    <row r="16" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B16" s="75"/>
       <c r="C16" s="64" t="s">
         <v>19</v>
@@ -1933,7 +2012,7 @@
       </c>
       <c r="Q16" s="32"/>
     </row>
-    <row r="17" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B17" s="75"/>
       <c r="C17" s="64" t="s">
         <v>19</v>
@@ -1979,7 +2058,7 @@
       </c>
       <c r="Q17" s="32"/>
     </row>
-    <row r="18" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="18" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B18" s="75"/>
       <c r="C18" s="64" t="s">
         <v>19</v>
@@ -2025,7 +2104,7 @@
       </c>
       <c r="Q18" s="32"/>
     </row>
-    <row r="19" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="19" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B19" s="65">
         <v>1</v>
       </c>
@@ -2073,7 +2152,7 @@
       </c>
       <c r="Q19" s="37"/>
     </row>
-    <row r="20" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B20" s="65">
         <v>1</v>
       </c>
@@ -2117,7 +2196,7 @@
       <c r="P20" s="42"/>
       <c r="Q20" s="43"/>
     </row>
-    <row r="21" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B21" s="65">
         <v>1</v>
       </c>
@@ -2165,7 +2244,7 @@
       </c>
       <c r="Q21" s="32"/>
     </row>
-    <row r="22" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B22" s="75">
         <v>9</v>
       </c>
@@ -2213,7 +2292,7 @@
       </c>
       <c r="Q22" s="27"/>
     </row>
-    <row r="23" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B23" s="75"/>
       <c r="C23" s="64" t="s">
         <v>17</v>
@@ -2259,7 +2338,7 @@
       </c>
       <c r="Q23" s="27"/>
     </row>
-    <row r="24" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B24" s="75"/>
       <c r="C24" s="64" t="s">
         <v>17</v>
@@ -2305,7 +2384,7 @@
       </c>
       <c r="Q24" s="27"/>
     </row>
-    <row r="25" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B25" s="75"/>
       <c r="C25" s="64" t="s">
         <v>17</v>
@@ -2351,7 +2430,7 @@
       </c>
       <c r="Q25" s="27"/>
     </row>
-    <row r="26" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B26" s="75"/>
       <c r="C26" s="64" t="s">
         <v>17</v>
@@ -2397,7 +2476,7 @@
       </c>
       <c r="Q26" s="27"/>
     </row>
-    <row r="27" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B27" s="75"/>
       <c r="C27" s="64" t="s">
         <v>17</v>
@@ -2443,7 +2522,7 @@
       </c>
       <c r="Q27" s="27"/>
     </row>
-    <row r="28" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B28" s="75"/>
       <c r="C28" s="64" t="s">
         <v>17</v>
@@ -2489,7 +2568,7 @@
       </c>
       <c r="Q28" s="27"/>
     </row>
-    <row r="29" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B29" s="75"/>
       <c r="C29" s="64" t="s">
         <v>17</v>
@@ -2535,7 +2614,7 @@
       </c>
       <c r="Q29" s="27"/>
     </row>
-    <row r="30" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B30" s="75"/>
       <c r="C30" s="64" t="s">
         <v>17</v>
@@ -2581,7 +2660,7 @@
       </c>
       <c r="Q30" s="27"/>
     </row>
-    <row r="31" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B31" s="75">
         <v>10</v>
       </c>
@@ -2629,7 +2708,7 @@
       </c>
       <c r="Q31" s="21"/>
     </row>
-    <row r="32" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B32" s="75"/>
       <c r="C32" s="64" t="s">
         <v>16</v>
@@ -2675,7 +2754,7 @@
       </c>
       <c r="Q32" s="21"/>
     </row>
-    <row r="33" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B33" s="75"/>
       <c r="C33" s="64" t="s">
         <v>16</v>
@@ -2721,7 +2800,7 @@
       </c>
       <c r="Q33" s="21"/>
     </row>
-    <row r="34" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B34" s="75"/>
       <c r="C34" s="64" t="s">
         <v>16</v>
@@ -2767,7 +2846,7 @@
       </c>
       <c r="Q34" s="21"/>
     </row>
-    <row r="35" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B35" s="75"/>
       <c r="C35" s="64" t="s">
         <v>16</v>
@@ -2813,7 +2892,7 @@
       </c>
       <c r="Q35" s="21"/>
     </row>
-    <row r="36" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B36" s="75"/>
       <c r="C36" s="64" t="s">
         <v>16</v>
@@ -2859,7 +2938,7 @@
       </c>
       <c r="Q36" s="21"/>
     </row>
-    <row r="37" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B37" s="75"/>
       <c r="C37" s="64" t="s">
         <v>16</v>
@@ -2905,7 +2984,7 @@
       </c>
       <c r="Q37" s="21"/>
     </row>
-    <row r="38" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B38" s="75"/>
       <c r="C38" s="64" t="s">
         <v>16</v>
@@ -2951,7 +3030,7 @@
       </c>
       <c r="Q38" s="21"/>
     </row>
-    <row r="39" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B39" s="75"/>
       <c r="C39" s="64" t="s">
         <v>16</v>
@@ -2997,7 +3076,7 @@
       </c>
       <c r="Q39" s="21"/>
     </row>
-    <row r="40" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B40" s="75"/>
       <c r="C40" s="64" t="s">
         <v>16</v>
@@ -3043,7 +3122,7 @@
       </c>
       <c r="Q40" s="21"/>
     </row>
-    <row r="41" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B41" s="75">
         <v>2</v>
       </c>
@@ -3089,7 +3168,7 @@
       <c r="P41" s="46"/>
       <c r="Q41" s="47"/>
     </row>
-    <row r="42" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B42" s="75"/>
       <c r="C42" s="64" t="s">
         <v>78</v>
@@ -3133,7 +3212,7 @@
       <c r="P42" s="46"/>
       <c r="Q42" s="47"/>
     </row>
-    <row r="43" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B43" s="65">
         <v>1</v>
       </c>
@@ -3181,7 +3260,7 @@
       </c>
       <c r="Q43" s="52"/>
     </row>
-    <row r="44" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B44" s="65">
         <v>1</v>
       </c>
@@ -3229,7 +3308,7 @@
       </c>
       <c r="Q44" s="43"/>
     </row>
-    <row r="45" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:17" x14ac:dyDescent="0.3">
       <c r="B45" s="65">
         <f>SUM(B5:B44)</f>
         <v>40</v>
@@ -3250,7 +3329,7 @@
       <c r="P45" s="67"/>
       <c r="Q45" s="57"/>
     </row>
-    <row r="46" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C46" s="15"/>
       <c r="D46" s="15"/>
       <c r="E46" s="15"/>
@@ -3266,7 +3345,7 @@
       <c r="O46" s="16"/>
       <c r="P46" s="17"/>
     </row>
-    <row r="47" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C47" s="15"/>
       <c r="D47" s="15"/>
       <c r="E47" s="15"/>
@@ -3282,7 +3361,7 @@
       <c r="O47" s="16"/>
       <c r="P47" s="17"/>
     </row>
-    <row r="48" spans="2:17" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:17" x14ac:dyDescent="0.3">
       <c r="C48" s="15"/>
       <c r="D48" s="15"/>
       <c r="E48" s="15"/>
@@ -3298,7 +3377,7 @@
       <c r="O48" s="16"/>
       <c r="P48" s="17"/>
     </row>
-    <row r="49" spans="3:16" x14ac:dyDescent="0.25">
+    <row r="49" spans="3:16" x14ac:dyDescent="0.3">
       <c r="C49" s="15"/>
       <c r="D49" s="15"/>
       <c r="E49" s="15"/>
@@ -3332,32 +3411,35 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4038A0F8-DC2D-4B1A-A07A-9A5B14662E1E}">
-  <dimension ref="B2:V17"/>
+  <dimension ref="B2:W24"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="K22" sqref="K22"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19:L19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="8" max="8" width="12.85546875" customWidth="1"/>
-    <col min="11" max="11" width="12.7109375" customWidth="1"/>
+    <col min="8" max="8" width="12.88671875" customWidth="1"/>
+    <col min="11" max="11" width="12.6640625" customWidth="1"/>
+    <col min="12" max="12" width="12.6640625" style="84" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B2" s="76" t="s">
-        <v>186</v>
-      </c>
-      <c r="C2" s="76"/>
-      <c r="D2" s="76"/>
-      <c r="E2" s="76"/>
-      <c r="F2" s="76"/>
-      <c r="G2" s="76"/>
-      <c r="H2" s="76"/>
-      <c r="I2" s="76"/>
-      <c r="J2" s="76"/>
-    </row>
-    <row r="3" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B2" s="74" t="s">
+        <v>231</v>
+      </c>
+      <c r="C2" s="74"/>
+      <c r="D2" s="74"/>
+      <c r="E2" s="74"/>
+      <c r="F2" s="74"/>
+      <c r="G2" s="74"/>
+      <c r="H2" s="74"/>
+      <c r="I2" s="74"/>
+      <c r="J2" s="74"/>
+      <c r="K2" s="74"/>
+      <c r="L2" s="74"/>
+    </row>
+    <row r="3" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B3" s="72"/>
       <c r="C3" s="72"/>
       <c r="D3" s="72"/>
@@ -3368,7 +3450,7 @@
       <c r="I3" s="72"/>
       <c r="J3" s="72"/>
     </row>
-    <row r="4" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="4" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B4" s="57"/>
       <c r="C4" s="57"/>
       <c r="D4" s="57"/>
@@ -3379,36 +3461,37 @@
       <c r="I4" s="57"/>
       <c r="J4" s="57"/>
       <c r="K4" s="57"/>
-      <c r="L4" s="81" t="s">
+      <c r="L4" s="85"/>
+      <c r="M4" s="76" t="s">
         <v>200</v>
       </c>
-      <c r="M4" s="81"/>
-      <c r="N4" s="81"/>
-      <c r="O4" s="81" t="s">
+      <c r="N4" s="76"/>
+      <c r="O4" s="76"/>
+      <c r="P4" s="76" t="s">
         <v>201</v>
       </c>
-      <c r="P4" s="81"/>
-      <c r="Q4" s="81" t="s">
+      <c r="Q4" s="76"/>
+      <c r="R4" s="76" t="s">
         <v>202</v>
       </c>
-      <c r="R4" s="81"/>
-      <c r="S4" s="81"/>
-      <c r="T4" s="81"/>
-      <c r="U4" s="56" t="s">
+      <c r="S4" s="76"/>
+      <c r="T4" s="76"/>
+      <c r="U4" s="76"/>
+      <c r="V4" s="56" t="s">
         <v>207</v>
       </c>
-      <c r="V4" s="56" t="s">
+      <c r="W4" s="56" t="s">
         <v>203</v>
       </c>
     </row>
-    <row r="5" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B5" s="73" t="s">
+    <row r="5" spans="2:23" s="72" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="B5" s="89" t="s">
         <v>28</v>
       </c>
-      <c r="C5" s="79" t="s">
+      <c r="C5" s="80" t="s">
         <v>0</v>
       </c>
-      <c r="D5" s="79"/>
+      <c r="D5" s="80"/>
       <c r="E5" s="58" t="s">
         <v>1</v>
       </c>
@@ -3427,50 +3510,53 @@
       <c r="J5" s="59" t="s">
         <v>26</v>
       </c>
-      <c r="K5" s="57" t="s">
+      <c r="K5" s="88" t="s">
         <v>70</v>
       </c>
-      <c r="L5" s="58" t="s">
+      <c r="L5" s="83" t="s">
+        <v>229</v>
+      </c>
+      <c r="M5" s="58" t="s">
         <v>187</v>
       </c>
-      <c r="M5" s="58" t="s">
+      <c r="N5" s="58" t="s">
         <v>188</v>
       </c>
-      <c r="N5" s="58" t="s">
+      <c r="O5" s="58" t="s">
         <v>189</v>
       </c>
-      <c r="O5" s="58" t="s">
+      <c r="P5" s="58" t="s">
         <v>190</v>
       </c>
-      <c r="P5" s="58" t="s">
+      <c r="Q5" s="58" t="s">
         <v>191</v>
       </c>
-      <c r="Q5" s="58" t="s">
+      <c r="R5" s="58" t="s">
         <v>192</v>
       </c>
-      <c r="R5" s="58" t="s">
+      <c r="S5" s="58" t="s">
         <v>194</v>
       </c>
-      <c r="S5" s="58" t="s">
+      <c r="T5" s="58" t="s">
         <v>195</v>
       </c>
-      <c r="T5" s="58" t="s">
+      <c r="U5" s="58" t="s">
         <v>196</v>
       </c>
-      <c r="U5" s="58" t="s">
+      <c r="V5" s="58" t="s">
         <v>209</v>
       </c>
-      <c r="V5" s="58" t="s">
+      <c r="W5" s="58" t="s">
         <v>193</v>
       </c>
     </row>
-    <row r="6" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B6" s="57"/>
-      <c r="C6" s="78" t="s">
+      <c r="C6" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="D6" s="78"/>
-      <c r="E6" s="78"/>
+      <c r="D6" s="79"/>
+      <c r="E6" s="79"/>
       <c r="F6" s="60" t="s">
         <v>8</v>
       </c>
@@ -3481,7 +3567,7 @@
         <v>10</v>
       </c>
       <c r="I6" s="60" t="s">
-        <v>11</v>
+        <v>233</v>
       </c>
       <c r="J6" s="61" t="s">
         <v>17</v>
@@ -3489,47 +3575,50 @@
       <c r="K6" s="57" t="s">
         <v>37</v>
       </c>
-      <c r="L6" s="60" t="s">
-        <v>8</v>
-      </c>
-      <c r="M6" s="57" t="s">
+      <c r="L6" s="87">
+        <v>5</v>
+      </c>
+      <c r="M6" s="60" t="s">
+        <v>8</v>
+      </c>
+      <c r="N6" s="57" t="s">
         <v>198</v>
       </c>
-      <c r="N6" s="57" t="s">
+      <c r="O6" s="57" t="s">
         <v>204</v>
       </c>
-      <c r="O6" s="63" t="s">
-        <v>54</v>
-      </c>
       <c r="P6" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="Q6" s="57" t="s">
+      <c r="Q6" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="R6" s="57" t="s">
         <v>199</v>
       </c>
-      <c r="R6" s="57" t="s">
+      <c r="S6" s="57" t="s">
         <v>205</v>
       </c>
-      <c r="S6" s="63" t="s">
-        <v>54</v>
-      </c>
-      <c r="T6" s="57" t="s">
+      <c r="T6" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="U6" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="U6" s="57" t="s">
+      <c r="V6" s="57" t="s">
         <v>206</v>
       </c>
-      <c r="V6" s="57" t="s">
+      <c r="W6" s="57" t="s">
         <v>197</v>
       </c>
     </row>
-    <row r="7" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B7" s="57"/>
-      <c r="C7" s="78" t="s">
+      <c r="C7" s="79" t="s">
         <v>23</v>
       </c>
-      <c r="D7" s="78"/>
-      <c r="E7" s="78"/>
+      <c r="D7" s="79"/>
+      <c r="E7" s="79"/>
       <c r="F7" s="60" t="s">
         <v>8</v>
       </c>
@@ -3540,7 +3629,7 @@
         <v>10</v>
       </c>
       <c r="I7" s="60" t="s">
-        <v>11</v>
+        <v>233</v>
       </c>
       <c r="J7" s="61" t="s">
         <v>17</v>
@@ -3548,20 +3637,20 @@
       <c r="K7" s="57" t="s">
         <v>44</v>
       </c>
-      <c r="L7" s="60" t="s">
-        <v>8</v>
-      </c>
-      <c r="M7" s="57" t="s">
+      <c r="L7" s="87">
+        <v>1</v>
+      </c>
+      <c r="M7" s="60" t="s">
+        <v>8</v>
+      </c>
+      <c r="N7" s="57" t="s">
         <v>198</v>
       </c>
-      <c r="N7" s="57" t="s">
+      <c r="O7" s="57" t="s">
         <v>204</v>
       </c>
-      <c r="O7" s="57"/>
       <c r="P7" s="57"/>
-      <c r="Q7" s="63" t="s">
-        <v>54</v>
-      </c>
+      <c r="Q7" s="57"/>
       <c r="R7" s="63" t="s">
         <v>54</v>
       </c>
@@ -3571,20 +3660,23 @@
       <c r="T7" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="U7" s="62" t="s">
+      <c r="U7" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="V7" s="62" t="s">
         <v>199</v>
       </c>
-      <c r="V7" s="57" t="s">
+      <c r="W7" s="57" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="8" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B8" s="57"/>
-      <c r="C8" s="78" t="s">
-        <v>23</v>
-      </c>
-      <c r="D8" s="78"/>
-      <c r="E8" s="78"/>
+      <c r="C8" s="79" t="s">
+        <v>235</v>
+      </c>
+      <c r="D8" s="79"/>
+      <c r="E8" s="79"/>
       <c r="F8" s="60" t="s">
         <v>8</v>
       </c>
@@ -3595,7 +3687,7 @@
         <v>10</v>
       </c>
       <c r="I8" s="60" t="s">
-        <v>11</v>
+        <v>233</v>
       </c>
       <c r="J8" s="61" t="s">
         <v>17</v>
@@ -3603,18 +3695,18 @@
       <c r="K8" s="57" t="s">
         <v>46</v>
       </c>
-      <c r="L8" s="60" t="s">
-        <v>8</v>
-      </c>
-      <c r="M8" s="57" t="s">
+      <c r="L8" s="87">
+        <v>9</v>
+      </c>
+      <c r="M8" s="60" t="s">
+        <v>8</v>
+      </c>
+      <c r="N8" s="57" t="s">
         <v>198</v>
       </c>
-      <c r="N8" s="57" t="s">
+      <c r="O8" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="O8" s="63" t="s">
-        <v>54</v>
-      </c>
       <c r="P8" s="63" t="s">
         <v>54</v>
       </c>
@@ -3630,19 +3722,22 @@
       <c r="T8" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="U8" s="57" t="s">
+      <c r="U8" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="V8" s="57" t="s">
         <v>206</v>
       </c>
-      <c r="V8" s="57" t="s">
+      <c r="W8" s="57" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="9" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B9" s="57"/>
-      <c r="C9" s="77" t="s">
+      <c r="C9" s="78" t="s">
         <v>24</v>
       </c>
-      <c r="D9" s="77"/>
+      <c r="D9" s="78"/>
       <c r="E9" s="1" t="s">
         <v>7</v>
       </c>
@@ -3655,8 +3750,8 @@
       <c r="H9" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="I9" s="1" t="s">
-        <v>11</v>
+      <c r="I9" s="60" t="s">
+        <v>233</v>
       </c>
       <c r="J9" s="55" t="s">
         <v>18</v>
@@ -3664,40 +3759,43 @@
       <c r="K9" s="1" t="s">
         <v>38</v>
       </c>
-      <c r="L9" s="57" t="s">
-        <v>8</v>
+      <c r="L9" s="87">
+        <v>3</v>
       </c>
       <c r="M9" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="N9" s="57" t="s">
         <v>198</v>
       </c>
-      <c r="N9" s="57" t="s">
+      <c r="O9" s="57" t="s">
         <v>204</v>
       </c>
-      <c r="O9" s="63" t="s">
-        <v>54</v>
-      </c>
       <c r="P9" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="Q9" s="57"/>
+      <c r="Q9" s="63" t="s">
+        <v>54</v>
+      </c>
       <c r="R9" s="57"/>
-      <c r="S9" s="57" t="s">
+      <c r="S9" s="57"/>
+      <c r="T9" s="57" t="s">
         <v>205</v>
       </c>
-      <c r="T9" s="57"/>
-      <c r="U9" s="57" t="s">
+      <c r="U9" s="57"/>
+      <c r="V9" s="57" t="s">
         <v>206</v>
       </c>
-      <c r="V9" s="57" t="s">
+      <c r="W9" s="57" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="10" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="10" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B10" s="57"/>
-      <c r="C10" s="77" t="s">
+      <c r="C10" s="78" t="s">
         <v>25</v>
       </c>
-      <c r="D10" s="77"/>
+      <c r="D10" s="78"/>
       <c r="E10" s="1" t="s">
         <v>7</v>
       </c>
@@ -3710,8 +3808,8 @@
       <c r="H10" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I10" s="1" t="s">
-        <v>11</v>
+      <c r="I10" s="60" t="s">
+        <v>233</v>
       </c>
       <c r="J10" s="55" t="s">
         <v>19</v>
@@ -3719,24 +3817,24 @@
       <c r="K10" s="1" t="s">
         <v>185</v>
       </c>
-      <c r="L10" s="57" t="s">
-        <v>8</v>
+      <c r="L10" s="87">
+        <v>6</v>
       </c>
       <c r="M10" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="N10" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="N10" s="57" t="s">
+      <c r="O10" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="O10" s="57" t="s">
+      <c r="P10" s="57" t="s">
         <v>208</v>
       </c>
-      <c r="P10" s="57" t="s">
+      <c r="Q10" s="57" t="s">
         <v>198</v>
       </c>
-      <c r="Q10" s="63" t="s">
-        <v>54</v>
-      </c>
       <c r="R10" s="63" t="s">
         <v>54</v>
       </c>
@@ -3746,20 +3844,23 @@
       <c r="T10" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="U10" s="57" t="s">
+      <c r="U10" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="V10" s="57" t="s">
         <v>210</v>
       </c>
-      <c r="V10" s="63" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="11" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="W10" s="63" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="11" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B11" s="57"/>
-      <c r="C11" s="80" t="s">
+      <c r="C11" s="81" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="80"/>
-      <c r="E11" s="80"/>
+      <c r="D11" s="81"/>
+      <c r="E11" s="81"/>
       <c r="F11" s="1" t="s">
         <v>8</v>
       </c>
@@ -3769,8 +3870,8 @@
       <c r="H11" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I11" s="1" t="s">
-        <v>11</v>
+      <c r="I11" s="60" t="s">
+        <v>233</v>
       </c>
       <c r="J11" s="55" t="s">
         <v>79</v>
@@ -3778,8 +3879,8 @@
       <c r="K11" s="1" t="s">
         <v>41</v>
       </c>
-      <c r="L11" s="63" t="s">
-        <v>54</v>
+      <c r="L11" s="87">
+        <v>1</v>
       </c>
       <c r="M11" s="63" t="s">
         <v>54</v>
@@ -3805,27 +3906,30 @@
       <c r="T11" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="U11" s="57" t="s">
+      <c r="U11" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="V11" s="57" t="s">
         <v>206</v>
       </c>
-      <c r="V11" s="63" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="12" spans="2:22" x14ac:dyDescent="0.25">
+      <c r="W11" s="63" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="12" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B12" s="57"/>
-      <c r="C12" s="77" t="s">
+      <c r="C12" s="78" t="s">
         <v>15</v>
       </c>
-      <c r="D12" s="77"/>
-      <c r="E12" s="77"/>
-      <c r="F12" s="77"/>
-      <c r="G12" s="77"/>
+      <c r="D12" s="78"/>
+      <c r="E12" s="78"/>
+      <c r="F12" s="78"/>
+      <c r="G12" s="78"/>
       <c r="H12" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I12" s="1" t="s">
-        <v>11</v>
+      <c r="I12" s="60" t="s">
+        <v>233</v>
       </c>
       <c r="J12" s="55" t="s">
         <v>21</v>
@@ -3833,8 +3937,8 @@
       <c r="K12" s="57" t="s">
         <v>43</v>
       </c>
-      <c r="L12" s="63" t="s">
-        <v>54</v>
+      <c r="L12" s="87">
+        <v>1</v>
       </c>
       <c r="M12" s="63" t="s">
         <v>54</v>
@@ -3842,15 +3946,15 @@
       <c r="N12" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="O12" s="57" t="s">
+      <c r="O12" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="P12" s="57" t="s">
         <v>208</v>
       </c>
-      <c r="P12" s="57" t="s">
+      <c r="Q12" s="57" t="s">
         <v>198</v>
       </c>
-      <c r="Q12" s="63" t="s">
-        <v>54</v>
-      </c>
       <c r="R12" s="63" t="s">
         <v>54</v>
       </c>
@@ -3860,19 +3964,22 @@
       <c r="T12" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="U12" s="57" t="s">
+      <c r="U12" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="V12" s="57" t="s">
         <v>210</v>
       </c>
-      <c r="V12" s="57" t="s">
+      <c r="W12" s="57" t="s">
         <v>206</v>
       </c>
     </row>
-    <row r="13" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B13" s="57"/>
-      <c r="C13" s="82" t="s">
+      <c r="C13" s="77" t="s">
         <v>6</v>
       </c>
-      <c r="D13" s="82"/>
+      <c r="D13" s="77"/>
       <c r="E13" s="1" t="s">
         <v>7</v>
       </c>
@@ -3885,8 +3992,8 @@
       <c r="H13" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I13" s="1" t="s">
-        <v>11</v>
+      <c r="I13" s="60" t="s">
+        <v>233</v>
       </c>
       <c r="J13" s="55" t="s">
         <v>16</v>
@@ -3894,18 +4001,18 @@
       <c r="K13" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="L13" s="57" t="s">
-        <v>8</v>
+      <c r="L13" s="87">
+        <v>10</v>
       </c>
       <c r="M13" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="N13" s="57" t="s">
         <v>7</v>
       </c>
-      <c r="N13" s="57" t="s">
+      <c r="O13" s="57" t="s">
         <v>11</v>
       </c>
-      <c r="O13" s="63" t="s">
-        <v>54</v>
-      </c>
       <c r="P13" s="63" t="s">
         <v>54</v>
       </c>
@@ -3921,20 +4028,23 @@
       <c r="T13" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="U13" s="57" t="s">
+      <c r="U13" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="V13" s="57" t="s">
         <v>206</v>
       </c>
-      <c r="V13" s="57" t="s">
+      <c r="W13" s="57" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="14" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B14" s="57"/>
-      <c r="C14" s="82" t="s">
+      <c r="C14" s="77" t="s">
         <v>80</v>
       </c>
-      <c r="D14" s="82"/>
-      <c r="E14" s="82"/>
+      <c r="D14" s="77"/>
+      <c r="E14" s="77"/>
       <c r="F14" s="1" t="s">
         <v>8</v>
       </c>
@@ -3944,8 +4054,8 @@
       <c r="H14" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I14" s="1" t="s">
-        <v>11</v>
+      <c r="I14" s="60" t="s">
+        <v>233</v>
       </c>
       <c r="J14" s="55" t="s">
         <v>78</v>
@@ -3953,8 +4063,8 @@
       <c r="K14" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="L14" s="63" t="s">
-        <v>54</v>
+      <c r="L14" s="87">
+        <v>2</v>
       </c>
       <c r="M14" s="63" t="s">
         <v>54</v>
@@ -3980,27 +4090,30 @@
       <c r="T14" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="U14" s="57" t="s">
+      <c r="U14" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="V14" s="57" t="s">
         <v>206</v>
       </c>
-      <c r="V14" s="63" t="s">
+      <c r="W14" s="63" t="s">
         <v>211</v>
       </c>
     </row>
-    <row r="15" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B15" s="57"/>
-      <c r="C15" s="77" t="s">
+      <c r="C15" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="D15" s="77"/>
-      <c r="E15" s="77"/>
-      <c r="F15" s="77"/>
-      <c r="G15" s="77"/>
+      <c r="D15" s="78"/>
+      <c r="E15" s="78"/>
+      <c r="F15" s="78"/>
+      <c r="G15" s="78"/>
       <c r="H15" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I15" s="1" t="s">
-        <v>11</v>
+      <c r="I15" s="60" t="s">
+        <v>233</v>
       </c>
       <c r="J15" s="55" t="s">
         <v>20</v>
@@ -4008,20 +4121,20 @@
       <c r="K15" s="1" t="s">
         <v>49</v>
       </c>
-      <c r="L15" s="57" t="s">
+      <c r="L15" s="87">
+        <v>1</v>
+      </c>
+      <c r="M15" s="57" t="s">
         <v>208</v>
       </c>
-      <c r="M15" s="57" t="s">
+      <c r="N15" s="57" t="s">
         <v>198</v>
       </c>
-      <c r="N15" s="57" t="s">
+      <c r="O15" s="57" t="s">
         <v>204</v>
       </c>
-      <c r="O15" s="57"/>
       <c r="P15" s="57"/>
-      <c r="Q15" s="63" t="s">
-        <v>54</v>
-      </c>
+      <c r="Q15" s="57"/>
       <c r="R15" s="63" t="s">
         <v>54</v>
       </c>
@@ -4031,27 +4144,30 @@
       <c r="T15" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="U15" s="57" t="s">
+      <c r="U15" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="V15" s="57" t="s">
         <v>206</v>
       </c>
-      <c r="V15" s="21" t="s">
+      <c r="W15" s="21" t="s">
         <v>210</v>
       </c>
     </row>
-    <row r="16" spans="2:22" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:23" x14ac:dyDescent="0.3">
       <c r="B16" s="57"/>
-      <c r="C16" s="77" t="s">
+      <c r="C16" s="78" t="s">
         <v>14</v>
       </c>
-      <c r="D16" s="77"/>
-      <c r="E16" s="77"/>
-      <c r="F16" s="77"/>
-      <c r="G16" s="77"/>
+      <c r="D16" s="78"/>
+      <c r="E16" s="78"/>
+      <c r="F16" s="78"/>
+      <c r="G16" s="78"/>
       <c r="H16" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="I16" s="1" t="s">
-        <v>11</v>
+      <c r="I16" s="60" t="s">
+        <v>233</v>
       </c>
       <c r="J16" s="55" t="s">
         <v>20</v>
@@ -4059,20 +4175,20 @@
       <c r="K16" s="1" t="s">
         <v>51</v>
       </c>
-      <c r="L16" s="57">
+      <c r="L16" s="87">
+        <v>1</v>
+      </c>
+      <c r="M16" s="57">
         <v>0</v>
       </c>
-      <c r="M16" s="57" t="s">
+      <c r="N16" s="57" t="s">
         <v>198</v>
       </c>
-      <c r="N16" s="57" t="s">
+      <c r="O16" s="57" t="s">
         <v>204</v>
       </c>
-      <c r="O16" s="57"/>
       <c r="P16" s="57"/>
-      <c r="Q16" s="63" t="s">
-        <v>54</v>
-      </c>
+      <c r="Q16" s="57"/>
       <c r="R16" s="63" t="s">
         <v>54</v>
       </c>
@@ -4082,15 +4198,18 @@
       <c r="T16" s="63" t="s">
         <v>54</v>
       </c>
-      <c r="U16" s="57" t="s">
+      <c r="U16" s="63" t="s">
+        <v>54</v>
+      </c>
+      <c r="V16" s="57" t="s">
         <v>206</v>
       </c>
-      <c r="V16" s="21" t="s">
+      <c r="W16" s="21" t="s">
         <v>199</v>
       </c>
     </row>
-    <row r="17" spans="2:22" x14ac:dyDescent="0.25">
-      <c r="B17" s="74" t="s">
+    <row r="17" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B17" s="73" t="s">
         <v>27</v>
       </c>
       <c r="C17" s="27">
@@ -4116,7 +4235,10 @@
       </c>
       <c r="J17" s="57"/>
       <c r="K17" s="57"/>
-      <c r="L17" s="57"/>
+      <c r="L17" s="87">
+        <f>SUM(L6:L16)</f>
+        <v>40</v>
+      </c>
       <c r="M17" s="57"/>
       <c r="N17" s="57"/>
       <c r="O17" s="57"/>
@@ -4127,15 +4249,143 @@
       <c r="T17" s="57"/>
       <c r="U17" s="57"/>
       <c r="V17" s="57"/>
+      <c r="W17" s="57"/>
+    </row>
+    <row r="19" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B19" s="93" t="s">
+        <v>230</v>
+      </c>
+      <c r="C19" s="94"/>
+      <c r="D19" s="94"/>
+      <c r="E19" s="94"/>
+      <c r="F19" s="94"/>
+      <c r="G19" s="94"/>
+      <c r="H19" s="94"/>
+      <c r="I19" s="94"/>
+      <c r="J19" s="94"/>
+      <c r="K19" s="94"/>
+      <c r="L19" s="94"/>
+    </row>
+    <row r="20" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B20" s="90"/>
+      <c r="C20" s="90"/>
+      <c r="D20" s="90"/>
+      <c r="E20" s="90"/>
+      <c r="F20" s="90"/>
+      <c r="G20" s="90"/>
+      <c r="H20" s="90"/>
+      <c r="I20" s="90"/>
+      <c r="J20" s="90"/>
+    </row>
+    <row r="21" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B21" s="57"/>
+      <c r="C21" s="57"/>
+      <c r="D21" s="57"/>
+      <c r="E21" s="57"/>
+      <c r="F21" s="57"/>
+      <c r="G21" s="57"/>
+      <c r="H21" s="57"/>
+      <c r="I21" s="57"/>
+      <c r="J21" s="57"/>
+      <c r="K21" s="57"/>
+      <c r="L21" s="85"/>
+    </row>
+    <row r="22" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B22" s="89" t="s">
+        <v>28</v>
+      </c>
+      <c r="C22" s="91" t="s">
+        <v>0</v>
+      </c>
+      <c r="D22" s="92"/>
+      <c r="E22" s="58" t="s">
+        <v>1</v>
+      </c>
+      <c r="F22" s="58" t="s">
+        <v>2</v>
+      </c>
+      <c r="G22" s="58" t="s">
+        <v>3</v>
+      </c>
+      <c r="H22" s="58" t="s">
+        <v>4</v>
+      </c>
+      <c r="I22" s="58" t="s">
+        <v>5</v>
+      </c>
+      <c r="J22" s="59" t="s">
+        <v>26</v>
+      </c>
+      <c r="K22" s="82" t="s">
+        <v>234</v>
+      </c>
+      <c r="L22" s="86" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="23" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B23" s="57"/>
+      <c r="C23" s="78" t="s">
+        <v>232</v>
+      </c>
+      <c r="D23" s="78"/>
+      <c r="E23" s="78"/>
+      <c r="F23" s="57" t="s">
+        <v>8</v>
+      </c>
+      <c r="G23" s="57" t="s">
+        <v>9</v>
+      </c>
+      <c r="H23" s="57" t="s">
+        <v>10</v>
+      </c>
+      <c r="I23" s="57" t="s">
+        <v>233</v>
+      </c>
+      <c r="J23" s="95" t="s">
+        <v>78</v>
+      </c>
+      <c r="K23" s="57" t="s">
+        <v>22</v>
+      </c>
+      <c r="L23" s="85">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="24" spans="2:23" x14ac:dyDescent="0.3">
+      <c r="B24" s="73" t="s">
+        <v>27</v>
+      </c>
+      <c r="C24" s="27">
+        <v>5</v>
+      </c>
+      <c r="D24" s="27">
+        <v>2</v>
+      </c>
+      <c r="E24" s="27">
+        <v>5</v>
+      </c>
+      <c r="F24" s="27">
+        <v>5</v>
+      </c>
+      <c r="G24" s="27">
+        <v>3</v>
+      </c>
+      <c r="H24" s="27">
+        <v>5</v>
+      </c>
+      <c r="I24" s="27">
+        <v>7</v>
+      </c>
+      <c r="J24" s="57"/>
+      <c r="K24" s="57"/>
+      <c r="L24" s="85"/>
     </row>
   </sheetData>
-  <mergeCells count="16">
-    <mergeCell ref="L4:N4"/>
-    <mergeCell ref="O4:P4"/>
-    <mergeCell ref="Q4:T4"/>
-    <mergeCell ref="C13:D13"/>
-    <mergeCell ref="C14:E14"/>
-    <mergeCell ref="B2:J2"/>
+  <mergeCells count="19">
+    <mergeCell ref="C22:D22"/>
+    <mergeCell ref="C23:E23"/>
+    <mergeCell ref="B19:L19"/>
     <mergeCell ref="C16:G16"/>
     <mergeCell ref="C6:E6"/>
     <mergeCell ref="C7:E7"/>
@@ -4146,6 +4396,12 @@
     <mergeCell ref="C10:D10"/>
     <mergeCell ref="C11:E11"/>
     <mergeCell ref="C12:G12"/>
+    <mergeCell ref="B2:L2"/>
+    <mergeCell ref="M4:O4"/>
+    <mergeCell ref="P4:Q4"/>
+    <mergeCell ref="R4:U4"/>
+    <mergeCell ref="C13:D13"/>
+    <mergeCell ref="C14:E14"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>